<commit_message>
fix template, add float input, add logo+name
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unusn\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unusn\ww\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7D90E6-8B19-40DF-A33D-FF604DCF3AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBC09FA-731D-4C1F-9D81-27CCA243118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13830" yWindow="1260" windowWidth="11820" windowHeight="11835" activeTab="1" xr2:uid="{E5890238-4733-4C84-BC7E-275D0E745093}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{E5890238-4733-4C84-BC7E-275D0E745093}"/>
   </bookViews>
   <sheets>
     <sheet name="DATAINPUT" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
   <si>
     <t>Bank Deposit Paper</t>
   </si>
@@ -201,9 +201,6 @@
     <t>UBER EATS / GRUBHUB FEE</t>
   </si>
   <si>
-    <t>AMEX</t>
-  </si>
-  <si>
     <t>OVER/SHORT</t>
   </si>
   <si>
@@ -217,18 +214,20 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Prepared by:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="165" formatCode="&quot; $&quot;#,##0.00&quot; &quot;;&quot; $(&quot;#,##0.00&quot;)&quot;;&quot; $-&quot;#&quot; &quot;"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,8 +289,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +359,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -375,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,8 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -421,46 +438,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -475,6 +458,56 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -817,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4889946A-F8EA-4B5F-816F-17A3D040DEC7}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,21 +862,25 @@
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
@@ -851,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -859,183 +896,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" s="26">
+        <v>0</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C5" s="26">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" s="26">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="15">
+      <c r="C7" s="26">
+        <v>0</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27">
         <f>SUM(C6,C7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="28">
+        <v>0</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="10">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" s="28">
+        <v>0</v>
+      </c>
+      <c r="D9" s="28">
         <f>SUM(C4,C5)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="29">
         <f>D9-C9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="10">
-        <v>0</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="28">
+        <v>0</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="28">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="10">
-        <v>0</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="10">
-        <v>0</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="10">
-        <v>0</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="28">
+        <v>0</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10">
-        <v>0</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
@@ -1044,11 +1081,11 @@
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="10">
-        <v>0</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="C17" s="28">
+        <v>0</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -1057,11 +1094,11 @@
       <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="11">
-        <v>0</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="30">
+        <v>0</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
@@ -1070,11 +1107,11 @@
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="11">
-        <v>0</v>
-      </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="C19" s="30">
+        <v>0</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -1083,11 +1120,11 @@
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="11">
-        <v>0</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="C20" s="30">
+        <v>0</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
@@ -1096,11 +1133,11 @@
       <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="12">
-        <v>0</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
+      <c r="C21" s="31">
+        <v>0</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
@@ -1109,11 +1146,11 @@
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="12">
-        <v>0</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
+      <c r="C22" s="31">
+        <v>0</v>
+      </c>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -1122,11 +1159,11 @@
       <c r="B23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="12">
-        <v>0</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="C23" s="31">
+        <v>0</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1135,505 +1172,540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2859EFBD-F18C-4A1C-88EC-DC3FF4BBD600}">
-  <dimension ref="B1:J31"/>
+  <dimension ref="B1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="0.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="1.140625" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="str">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="str">
         <f>DATAINPUT!D1</f>
         <v>CR</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25">
         <f>DATAINPUT!B2</f>
         <v>0</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2" s="21">
         <f>DATAINPUT!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="35"/>
-    </row>
-    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+      <c r="J5" s="32"/>
+    </row>
+    <row r="6" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="34">
         <f>C24</f>
         <v>0</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="34">
         <f>DATAINPUT!C18</f>
         <v>0</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="34">
         <f>DATAINPUT!C21</f>
         <v>0</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="36">
         <f>+F6+G6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="19" t="s">
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="16"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="34">
         <f>DATAINPUT!C19</f>
         <v>0</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="34">
         <f>DATAINPUT!C22</f>
         <v>0</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="36">
         <f>+F7+G7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="19" t="s">
+      <c r="J7" s="32"/>
+    </row>
+    <row r="8" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="17"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="21"/>
-    </row>
-    <row r="9" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="19" t="s">
+      <c r="G8" s="41"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="32"/>
+    </row>
+    <row r="9" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="21" t="s">
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="J9" s="32"/>
+    </row>
+    <row r="10" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="21"/>
-    </row>
-    <row r="11" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+      <c r="H10" s="36"/>
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="37">
         <f>DATAINPUT!C12</f>
         <v>0</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-    </row>
-    <row r="12" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="J11" s="32"/>
+    </row>
+    <row r="12" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="34">
         <f>DATAINPUT!C13</f>
         <v>0</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-    </row>
-    <row r="13" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="34">
         <f>DATAINPUT!C10</f>
         <v>0</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="J13" s="32"/>
+    </row>
+    <row r="14" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="37">
         <f>DATAINPUT!C11</f>
         <v>0</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="24">
+      <c r="F14" s="36"/>
+      <c r="G14" s="37">
         <f>DATAINPUT!C15</f>
         <v>0</v>
       </c>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19" t="s">
+      <c r="H14" s="36"/>
+      <c r="J14" s="32"/>
+    </row>
+    <row r="15" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="34">
         <f>DATAINPUT!C14</f>
         <v>0</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="25">
+      <c r="D15" s="15"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="42">
         <f>DATAINPUT!C25</f>
         <v>0</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="H15" s="36"/>
+      <c r="J15" s="32"/>
+    </row>
+    <row r="16" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="17"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="19" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="34">
         <f>DATAINPUT!C20</f>
         <v>0</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="34">
         <f>DATAINPUT!C23</f>
         <v>0</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="36">
         <f>SUM(F17:G17)</f>
         <v>0</v>
       </c>
+      <c r="J17" s="32"/>
     </row>
     <row r="18" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="19" t="s">
+      <c r="B19" s="16"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="34">
         <f>DATAINPUT!C6</f>
         <v>0</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="34">
         <f>DATAINPUT!C7</f>
         <v>0</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="36">
         <f>SUM(F19:G19)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="J19" s="32"/>
+    </row>
+    <row r="20" spans="2:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="36">
         <f>SUM(C6:C19)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="21">
+      <c r="D20" s="15"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="36">
         <f>SUM(F6:F9,F12)-F13-F14-F15+F17+F19</f>
         <v>0</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="36">
         <f>SUM(G6:G9,G12)-G13-G14-G15+G17+G19</f>
         <v>0</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="36">
         <f>F20+G20</f>
         <v>0</v>
       </c>
       <c r="J20" s="33">
-        <f>C20-H20</f>
+        <f>H20-C20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="J21" s="32"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="38">
         <f>DATAINPUT!C9</f>
         <v>0</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="19" t="s">
+      <c r="D23" s="15"/>
+      <c r="E23" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="24">
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="37">
         <f>DATAINPUT!C8+DATAINPUT!C16+DATAINPUT!C17</f>
         <v>0</v>
       </c>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="37">
         <f>DATAINPUT!D9</f>
         <v>0</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="19" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="24">
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="37">
         <f>DATAINPUT!C17</f>
         <v>0</v>
       </c>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="39">
         <f>C24-C23</f>
         <v>0</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="19" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="24">
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="37">
         <f>DATAINPUT!C16</f>
         <v>0</v>
       </c>
+      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="19"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="19" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="29">
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="43">
         <f>H23-SUM(H24:H25)</f>
         <v>0</v>
       </c>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="2:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="31" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="24">
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="37">
         <f>DATAINPUT!C15</f>
         <v>0</v>
       </c>
+      <c r="J27" s="32"/>
     </row>
     <row r="28" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="36">
+        <f>H26-H27</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="27" t="s">
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="36">
+        <f>H19</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" spans="2:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="21">
-        <f>H26-H27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="21">
-        <f>H19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="19" t="s">
+      <c r="H30" s="36">
+        <f>H28+H29</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="33">
+        <f>H30-H20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="45" t="str">
+        <f>DATAINPUT!B1</f>
+        <v>CR</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="H30" s="21">
-        <f>H28+H29</f>
-        <v>0</v>
-      </c>
-      <c r="J30" s="33">
-        <f>H20-H30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="21">
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="36">
         <f>C20</f>
         <v>0</v>
       </c>
+      <c r="J31" s="32"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="32"/>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="32"/>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="32"/>
+    </row>
+    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1645,5 +1717,6 @@
     <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>